<commit_message>
The sending data to MongoDB Server functionality implemented and added new test cases
</commit_message>
<xml_diff>
--- a/TestingGuides/ProjectGantt.xlsx
+++ b/TestingGuides/ProjectGantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\college\year4\FYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\college\year4\TestingGuides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5126E5-070D-4177-97AF-9CFB21FA9E0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD7C6EF-4927-47E9-BE6C-891A44C3FB5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,6 +617,9 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -664,9 +667,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1079,14 +1079,14 @@
   </sheetPr>
   <dimension ref="B1:BO34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="2" customWidth="1"/>
     <col min="3" max="5" width="11.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
@@ -1105,13 +1105,13 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1119,66 +1119,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="37"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="34" t="s">
+      <c r="Q2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="36"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="38"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="39"/>
       <c r="Z2" s="17"/>
-      <c r="AA2" s="39" t="s">
+      <c r="AA2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="42"/>
       <c r="AH2" s="18"/>
-      <c r="AI2" s="26" t="s">
+      <c r="AI2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="34" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="19" t="s">
@@ -1205,12 +1205,12 @@
       <c r="AA3" s="9"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="30"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:67" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B16" s="20" t="s">
         <v>40</v>
       </c>
@@ -1632,8 +1632,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="42" t="s">
+    <row r="17" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="B17" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="23">
@@ -1652,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="52.2" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
         <v>26</v>
       </c>

</xml_diff>